<commit_message>
Update Usabiluty.xlsx, have all except set playlists
</commit_message>
<xml_diff>
--- a/iSpring/Usabiluty.xlsx
+++ b/iSpring/Usabiluty.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="254" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="166">
   <si>
     <t>Изменение заголовка слайда</t>
   </si>
@@ -472,9 +472,6 @@
     <t>Нажать OK</t>
   </si>
   <si>
-    <t>В ячейке столба Branching отображается переход только на следующий слайд</t>
-  </si>
-  <si>
     <t>Выбор докладчика</t>
   </si>
   <si>
@@ -497,6 +494,30 @@
   </si>
   <si>
     <t>Название layout отображается над картинкой layout</t>
+  </si>
+  <si>
+    <t>Смена playlist  у слайда</t>
+  </si>
+  <si>
+    <t>Нажать в столбце Playlist в центр ячейки</t>
+  </si>
+  <si>
+    <t>Выбрать из списка playlist</t>
+  </si>
+  <si>
+    <t>Название playlist отображается в центре ячейки</t>
+  </si>
+  <si>
+    <t>В ячейке столба Branching отображается переход только на следующий слайд, отображается посередине ячейки</t>
+  </si>
+  <si>
+    <t>Выбрать слайд</t>
+  </si>
+  <si>
+    <t>Нажать на кнопку в ленте в разделе Display Slides на Hide slide</t>
+  </si>
+  <si>
+    <t>Над слайдом появится надпись hidden, она будет четко видна, отображается в центре слайда, кнопка Hide slide четко выделена и это хорошо видно</t>
   </si>
 </sst>
 </file>
@@ -826,7 +847,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="82">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -994,7 +1015,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1030,14 +1057,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="5">
@@ -1552,8 +1588,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView topLeftCell="A47" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47:D47"/>
+    <sheetView topLeftCell="A77" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59:D59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2635,10 +2671,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E15"/>
+  <dimension ref="A2:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14:D15"/>
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2675,10 +2711,10 @@
       <c r="B4" s="60" t="s">
         <v>137</v>
       </c>
-      <c r="C4" s="69" t="s">
+      <c r="C4" s="71" t="s">
         <v>142</v>
       </c>
-      <c r="D4" s="67" t="s">
+      <c r="D4" s="68" t="s">
         <v>142</v>
       </c>
     </row>
@@ -2687,124 +2723,174 @@
       <c r="B5" s="65" t="s">
         <v>138</v>
       </c>
-      <c r="C5" s="70"/>
-      <c r="D5" s="68"/>
+      <c r="C5" s="72"/>
+      <c r="D5" s="70"/>
     </row>
     <row r="6" spans="1:5" ht="45" customHeight="1">
-      <c r="A6" s="71" t="s">
+      <c r="A6" s="73" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="72" t="s">
+      <c r="B6" s="74" t="s">
         <v>139</v>
       </c>
       <c r="C6" s="61" t="s">
         <v>141</v>
       </c>
-      <c r="D6" s="67" t="s">
+      <c r="D6" s="68" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="7" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A7" s="73"/>
+      <c r="A7" s="75"/>
       <c r="B7" s="65" t="s">
         <v>140</v>
       </c>
       <c r="C7" s="66"/>
-      <c r="D7" s="68"/>
+      <c r="D7" s="70"/>
     </row>
     <row r="8" spans="1:5" ht="48.75" customHeight="1" thickBot="1">
-      <c r="A8" s="74" t="s">
+      <c r="A8" s="76" t="s">
         <v>143</v>
       </c>
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="77" t="s">
         <v>144</v>
       </c>
-      <c r="C8" s="76" t="s">
+      <c r="C8" s="78" t="s">
         <v>145</v>
       </c>
-      <c r="D8" s="77" t="s">
+      <c r="D8" s="79" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="30">
-      <c r="A9" s="71" t="s">
+    <row r="9" spans="1:5" ht="30" customHeight="1">
+      <c r="A9" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="72" t="s">
+      <c r="B9" s="82" t="s">
         <v>147</v>
       </c>
       <c r="C9" s="61" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="67" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="30">
+      <c r="A10" s="80"/>
+      <c r="B10" s="83" t="s">
+        <v>148</v>
+      </c>
+      <c r="C10" s="62"/>
+      <c r="D10" s="81"/>
+    </row>
+    <row r="11" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A11" s="75"/>
+      <c r="B11" s="84" t="s">
+        <v>149</v>
+      </c>
+      <c r="C11" s="66"/>
+      <c r="D11" s="69"/>
+    </row>
+    <row r="12" spans="1:5" ht="30">
+      <c r="A12" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="D9" s="67" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="30">
-      <c r="A10" s="78"/>
-      <c r="B10" s="39" t="s">
-        <v>148</v>
-      </c>
-      <c r="C10" s="62"/>
-      <c r="D10" s="79"/>
-    </row>
-    <row r="11" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A11" s="73"/>
-      <c r="B11" s="65" t="s">
-        <v>149</v>
-      </c>
-      <c r="C11" s="66"/>
-      <c r="D11" s="68"/>
-    </row>
-    <row r="12" spans="1:5" ht="30">
-      <c r="A12" s="71" t="s">
+      <c r="B12" s="85" t="s">
         <v>151</v>
       </c>
-      <c r="B12" s="80" t="s">
+      <c r="C12" s="61" t="s">
+        <v>153</v>
+      </c>
+      <c r="D12" s="68" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A13" s="75"/>
+      <c r="B13" s="86" t="s">
         <v>152</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C13" s="66"/>
+      <c r="D13" s="70"/>
+    </row>
+    <row r="14" spans="1:5" ht="30">
+      <c r="A14" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="D12" s="67" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A13" s="73"/>
-      <c r="B13" s="81" t="s">
-        <v>153</v>
-      </c>
-      <c r="C13" s="66"/>
-      <c r="D13" s="68"/>
-    </row>
-    <row r="14" spans="1:5" ht="30">
-      <c r="A14" s="71" t="s">
+      <c r="B14" s="85" t="s">
         <v>155</v>
       </c>
-      <c r="B14" s="80" t="s">
+      <c r="C14" s="61" t="s">
+        <v>157</v>
+      </c>
+      <c r="D14" s="68" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A15" s="75"/>
+      <c r="B15" s="86" t="s">
         <v>156</v>
       </c>
-      <c r="C14" s="61" t="s">
+      <c r="C15" s="66"/>
+      <c r="D15" s="70"/>
+    </row>
+    <row r="16" spans="1:5" ht="30">
+      <c r="A16" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="D14" s="67" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" ht="15.75" thickBot="1">
-      <c r="A15" s="73"/>
-      <c r="B15" s="81" t="s">
-        <v>157</v>
-      </c>
-      <c r="C15" s="66"/>
-      <c r="D15" s="68"/>
+      <c r="B16" s="85" t="s">
+        <v>159</v>
+      </c>
+      <c r="C16" s="61" t="s">
+        <v>161</v>
+      </c>
+      <c r="D16" s="68" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A17" s="75"/>
+      <c r="B17" s="86" t="s">
+        <v>160</v>
+      </c>
+      <c r="C17" s="66"/>
+      <c r="D17" s="70"/>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" s="73" t="s">
+        <v>10</v>
+      </c>
+      <c r="B18" s="85" t="s">
+        <v>163</v>
+      </c>
+      <c r="C18" s="61" t="s">
+        <v>165</v>
+      </c>
+      <c r="D18" s="68" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="51.75" customHeight="1" thickBot="1">
+      <c r="A19" s="75"/>
+      <c r="B19" s="86" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="66"/>
+      <c r="D19" s="70"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="21">
+    <mergeCell ref="D18:D19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="A18:A19"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="A14:A15"/>
+    <mergeCell ref="C16:C17"/>
+    <mergeCell ref="D16:D17"/>
+    <mergeCell ref="A16:A17"/>
     <mergeCell ref="A9:A11"/>
     <mergeCell ref="C9:C11"/>
     <mergeCell ref="D9:D11"/>

</xml_diff>

<commit_message>
Usability almost ready, remained comments
</commit_message>
<xml_diff>
--- a/iSpring/Usabiluty.xlsx
+++ b/iSpring/Usabiluty.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="264" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="176">
   <si>
     <t>Изменение заголовка слайда</t>
   </si>
@@ -518,6 +518,36 @@
   </si>
   <si>
     <t>Над слайдом появится надпись hidden, она будет четко видна, отображается в центре слайда, кнопка Hide slide четко выделена и это хорошо видно</t>
+  </si>
+  <si>
+    <t>Поиск редактора playlist</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нажать в ленте в разделе Advanced на playlist </t>
+  </si>
+  <si>
+    <t>В выпадающем списке выбрать Manage playlist…</t>
+  </si>
+  <si>
+    <t>Manage playlist… находится в конце списка и отделён от имеющихся playlist линией</t>
+  </si>
+  <si>
+    <t>Редактирование списка playlist</t>
+  </si>
+  <si>
+    <t>Добавить новый</t>
+  </si>
+  <si>
+    <t>Добавить в него звуки</t>
+  </si>
+  <si>
+    <t>Переместить несколько из них в списке</t>
+  </si>
+  <si>
+    <t>Удалить один из звуков</t>
+  </si>
+  <si>
+    <t>Кнопки сгруппированы. Отдельно стоят кнопки редактирования списков playlist и редактирования списка звуков. Кнопки перемещения звуков в одной группе, удаления и добавления в другой.  Кнопки перемещения вверх расположена над кнопкой перемещения вниз.</t>
   </si>
 </sst>
 </file>
@@ -847,7 +877,7 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="89">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1060,6 +1090,9 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
@@ -1073,6 +1106,9 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1588,7 +1624,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:D102"/>
   <sheetViews>
-    <sheetView topLeftCell="A77" workbookViewId="0">
+    <sheetView topLeftCell="A62" workbookViewId="0">
       <selection activeCell="B59" sqref="B59:D59"/>
     </sheetView>
   </sheetViews>
@@ -2671,10 +2707,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:E19"/>
+  <dimension ref="A2:E25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -2766,7 +2802,7 @@
       <c r="A9" s="73" t="s">
         <v>146</v>
       </c>
-      <c r="B9" s="82" t="s">
+      <c r="B9" s="83" t="s">
         <v>147</v>
       </c>
       <c r="C9" s="61" t="s">
@@ -2778,7 +2814,7 @@
     </row>
     <row r="10" spans="1:5" ht="30">
       <c r="A10" s="80"/>
-      <c r="B10" s="83" t="s">
+      <c r="B10" s="84" t="s">
         <v>148</v>
       </c>
       <c r="C10" s="62"/>
@@ -2786,7 +2822,7 @@
     </row>
     <row r="11" spans="1:5" ht="15.75" thickBot="1">
       <c r="A11" s="75"/>
-      <c r="B11" s="84" t="s">
+      <c r="B11" s="85" t="s">
         <v>149</v>
       </c>
       <c r="C11" s="66"/>
@@ -2796,7 +2832,7 @@
       <c r="A12" s="73" t="s">
         <v>150</v>
       </c>
-      <c r="B12" s="85" t="s">
+      <c r="B12" s="86" t="s">
         <v>151</v>
       </c>
       <c r="C12" s="61" t="s">
@@ -2808,7 +2844,7 @@
     </row>
     <row r="13" spans="1:5" ht="15.75" thickBot="1">
       <c r="A13" s="75"/>
-      <c r="B13" s="86" t="s">
+      <c r="B13" s="87" t="s">
         <v>152</v>
       </c>
       <c r="C13" s="66"/>
@@ -2818,7 +2854,7 @@
       <c r="A14" s="73" t="s">
         <v>154</v>
       </c>
-      <c r="B14" s="85" t="s">
+      <c r="B14" s="86" t="s">
         <v>155</v>
       </c>
       <c r="C14" s="61" t="s">
@@ -2830,7 +2866,7 @@
     </row>
     <row r="15" spans="1:5" ht="15.75" thickBot="1">
       <c r="A15" s="75"/>
-      <c r="B15" s="86" t="s">
+      <c r="B15" s="87" t="s">
         <v>156</v>
       </c>
       <c r="C15" s="66"/>
@@ -2840,7 +2876,7 @@
       <c r="A16" s="73" t="s">
         <v>158</v>
       </c>
-      <c r="B16" s="85" t="s">
+      <c r="B16" s="86" t="s">
         <v>159</v>
       </c>
       <c r="C16" s="61" t="s">
@@ -2852,7 +2888,7 @@
     </row>
     <row r="17" spans="1:4" ht="15.75" thickBot="1">
       <c r="A17" s="75"/>
-      <c r="B17" s="86" t="s">
+      <c r="B17" s="87" t="s">
         <v>160</v>
       </c>
       <c r="C17" s="66"/>
@@ -2862,7 +2898,7 @@
       <c r="A18" s="73" t="s">
         <v>10</v>
       </c>
-      <c r="B18" s="85" t="s">
+      <c r="B18" s="86" t="s">
         <v>163</v>
       </c>
       <c r="C18" s="61" t="s">
@@ -2874,17 +2910,83 @@
     </row>
     <row r="19" spans="1:4" ht="51.75" customHeight="1" thickBot="1">
       <c r="A19" s="75"/>
-      <c r="B19" s="86" t="s">
+      <c r="B19" s="87" t="s">
         <v>164</v>
       </c>
       <c r="C19" s="66"/>
       <c r="D19" s="70"/>
     </row>
+    <row r="20" spans="1:4" ht="30">
+      <c r="A20" s="63" t="s">
+        <v>166</v>
+      </c>
+      <c r="B20" s="86" t="s">
+        <v>167</v>
+      </c>
+      <c r="C20" s="61" t="s">
+        <v>169</v>
+      </c>
+      <c r="D20" s="68" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="30.75" thickBot="1">
+      <c r="A21" s="64"/>
+      <c r="B21" s="87" t="s">
+        <v>168</v>
+      </c>
+      <c r="C21" s="66"/>
+      <c r="D21" s="70"/>
+    </row>
+    <row r="22" spans="1:4" ht="15" customHeight="1">
+      <c r="A22" s="73" t="s">
+        <v>170</v>
+      </c>
+      <c r="B22" s="86" t="s">
+        <v>171</v>
+      </c>
+      <c r="C22" s="61" t="s">
+        <v>175</v>
+      </c>
+      <c r="D22" s="68" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="36.75" customHeight="1">
+      <c r="A23" s="80"/>
+      <c r="B23" s="88" t="s">
+        <v>172</v>
+      </c>
+      <c r="C23" s="62"/>
+      <c r="D23" s="82"/>
+    </row>
+    <row r="24" spans="1:4" ht="45" customHeight="1">
+      <c r="A24" s="80"/>
+      <c r="B24" s="88" t="s">
+        <v>173</v>
+      </c>
+      <c r="C24" s="62"/>
+      <c r="D24" s="82"/>
+    </row>
+    <row r="25" spans="1:4" ht="44.25" customHeight="1" thickBot="1">
+      <c r="A25" s="75"/>
+      <c r="B25" s="87" t="s">
+        <v>174</v>
+      </c>
+      <c r="C25" s="66"/>
+      <c r="D25" s="70"/>
+    </row>
   </sheetData>
-  <mergeCells count="21">
+  <mergeCells count="27">
+    <mergeCell ref="C22:C25"/>
+    <mergeCell ref="A22:A25"/>
+    <mergeCell ref="D22:D25"/>
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="C18:C19"/>
     <mergeCell ref="A18:A19"/>
+    <mergeCell ref="C20:C21"/>
+    <mergeCell ref="D20:D21"/>
+    <mergeCell ref="A20:A21"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="A14:A15"/>

</xml_diff>